<commit_message>
updated meeting minutes updated to final meeting minutes
</commit_message>
<xml_diff>
--- a/Meeting Minutes and Questions/Final Meeting Minutes.xlsx
+++ b/Meeting Minutes and Questions/Final Meeting Minutes.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moura\DLP_CW\Meeting Minutes and Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E9BFA63-BFA6-4B9D-865A-1B77D2615BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A133B7E-39DB-4E7A-8054-AA73AF0E7D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -310,9 +323,6 @@
 - Discussed clustering model</t>
   </si>
   <si>
-    <t>-Finish resole cleaning and assit Rawad if required with the dataset avaliable</t>
-  </si>
-  <si>
     <t>- Logged feedback for meeting with Phil
 - Discussed clustering model</t>
   </si>
@@ -469,6 +479,9 @@
   <si>
     <t>- Understanded the other datasets provided
 - I helped Bhavjot with the durations of the planning phase and the WBS</t>
+  </si>
+  <si>
+    <t>-Finished resole cleaning and assit Rawad if required with the dataset avaliable</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1364,6 +1377,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1629,8 +1645,8 @@
   </sheetPr>
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1961,7 +1977,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E27" s="64" t="s">
         <v>52</v>
@@ -2020,7 +2036,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E32" s="66" t="s">
         <v>59</v>
@@ -2211,8 +2227,8 @@
       <c r="D47" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="14" t="s">
-        <v>83</v>
+      <c r="E47" s="67" t="s">
+        <v>131</v>
       </c>
       <c r="F47" s="31"/>
     </row>
@@ -2222,13 +2238,13 @@
         <v>16</v>
       </c>
       <c r="D48" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="F48" s="32" t="s">
         <v>85</v>
-      </c>
-      <c r="F48" s="32" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2237,10 +2253,10 @@
         <v>19</v>
       </c>
       <c r="D49" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>88</v>
       </c>
       <c r="F49" s="21"/>
     </row>
@@ -2270,10 +2286,10 @@
         <v>13</v>
       </c>
       <c r="D52" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="F52" s="32"/>
     </row>
@@ -2283,13 +2299,13 @@
         <v>16</v>
       </c>
       <c r="D53" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="F53" s="31" t="s">
         <v>92</v>
-      </c>
-      <c r="F53" s="31" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2309,10 +2325,10 @@
         <v>7</v>
       </c>
       <c r="D55" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>95</v>
       </c>
       <c r="F55" s="10"/>
     </row>
@@ -2330,11 +2346,11 @@
       <c r="C57" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D57" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="E57" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>97</v>
       </c>
       <c r="F57" s="31"/>
     </row>
@@ -2344,10 +2360,10 @@
         <v>16</v>
       </c>
       <c r="D58" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E58" s="13" t="s">
         <v>98</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>99</v>
       </c>
       <c r="F58" s="32"/>
     </row>
@@ -2362,7 +2378,7 @@
     </row>
     <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B60" s="53">
         <v>45736</v>
@@ -2371,10 +2387,10 @@
         <v>7</v>
       </c>
       <c r="D60" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="E60" s="56" t="s">
         <v>101</v>
-      </c>
-      <c r="E60" s="56" t="s">
-        <v>102</v>
       </c>
       <c r="F60" s="56"/>
     </row>
@@ -2393,7 +2409,7 @@
         <v>13</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E62" s="13"/>
       <c r="F62" s="32"/>
@@ -2404,7 +2420,7 @@
         <v>16</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E63" s="16"/>
       <c r="F63" s="31"/>
@@ -2426,7 +2442,7 @@
         <v>7</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="10"/>
@@ -2437,10 +2453,10 @@
         <v>10</v>
       </c>
       <c r="D66" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E66" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>107</v>
       </c>
       <c r="F66" s="32"/>
     </row>
@@ -2450,7 +2466,7 @@
         <v>13</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E67" s="16"/>
       <c r="F67" s="31"/>
@@ -2461,7 +2477,7 @@
         <v>16</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E68" s="13"/>
       <c r="F68" s="32"/>
@@ -2472,14 +2488,14 @@
         <v>19</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="21"/>
     </row>
     <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B70" s="22">
         <v>45740</v>
@@ -2497,7 +2513,7 @@
         <v>10</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E71" s="16"/>
       <c r="F71" s="31"/>
@@ -2508,10 +2524,10 @@
         <v>13</v>
       </c>
       <c r="D72" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E72" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="F72" s="32"/>
     </row>
@@ -2521,10 +2537,10 @@
         <v>16</v>
       </c>
       <c r="D73" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E73" s="16" t="s">
         <v>114</v>
-      </c>
-      <c r="E73" s="16" t="s">
-        <v>115</v>
       </c>
       <c r="F73" s="31"/>
     </row>
@@ -2534,10 +2550,10 @@
         <v>19</v>
       </c>
       <c r="D74" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E74" s="13" t="s">
         <v>116</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>117</v>
       </c>
       <c r="F74" s="32"/>
     </row>
@@ -2549,10 +2565,10 @@
         <v>7</v>
       </c>
       <c r="D75" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="E75" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="F75" s="10"/>
     </row>
@@ -2562,7 +2578,7 @@
         <v>10</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E76" s="13"/>
       <c r="F76" s="32"/>
@@ -2573,10 +2589,10 @@
         <v>13</v>
       </c>
       <c r="D77" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E77" s="16" t="s">
         <v>121</v>
-      </c>
-      <c r="E77" s="16" t="s">
-        <v>122</v>
       </c>
       <c r="F77" s="31"/>
     </row>
@@ -2586,13 +2602,13 @@
         <v>16</v>
       </c>
       <c r="D78" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E78" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E78" s="13" t="s">
+      <c r="F78" s="32" t="s">
         <v>124</v>
-      </c>
-      <c r="F78" s="32" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2601,16 +2617,16 @@
         <v>19</v>
       </c>
       <c r="D79" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E79" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="E79" s="16" t="s">
-        <v>127</v>
       </c>
       <c r="F79" s="31"/>
     </row>
     <row r="80" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B80" s="59">
         <v>45690</v>
@@ -2619,7 +2635,7 @@
         <v>19</v>
       </c>
       <c r="D80" s="61" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E80" s="61"/>
       <c r="F80" s="62"/>

</xml_diff>